<commit_message>
WORK IN PROGRESS. NIGHTLY COMMIT. Minor updates to appliance input data.
</commit_message>
<xml_diff>
--- a/bcd/CREST/Appliance/Appliance_Characteristics.xlsx
+++ b/bcd/CREST/Appliance/Appliance_Characteristics.xlsx
@@ -582,23 +582,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -621,6 +609,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2880,11 +2880,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113190400"/>
-        <c:axId val="113188864"/>
+        <c:axId val="64158336"/>
+        <c:axId val="64512384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113190400"/>
+        <c:axId val="64158336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="365"/>
@@ -2896,12 +2896,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113188864"/>
+        <c:crossAx val="64512384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113188864"/>
+        <c:axId val="64512384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,14 +2912,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113190400"/>
+        <c:crossAx val="64158336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3260,7 +3259,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3619,95 +3618,95 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="29">
         <v>1500</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="26">
         <v>0</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="30">
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="32">
         <v>120</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="32">
         <v>4</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33">
+      <c r="E12" s="29"/>
+      <c r="F12" s="29">
         <v>449</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="26">
         <f t="shared" si="2"/>
         <v>37.416666666666664</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="30">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3785,33 +3784,33 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="27">
         <v>11000</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="28">
         <v>0</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="30">
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4084,7 +4083,7 @@
       <c r="E24" s="5">
         <v>5</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>864</v>
       </c>
       <c r="G24">
@@ -4099,7 +4098,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="4">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -4116,6 +4115,22 @@
       </c>
       <c r="D25" s="14">
         <v>1</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" ref="G25" si="4">F25/12</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" ref="H25" si="5">(C25/1000)*(E25/60)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" ref="I25" si="6">(G25*E25)/60</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" ref="J25" si="7">H25*G25</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -7493,64 +7508,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:14" s="11" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="H2" s="21" t="s">
+      <c r="F2" s="21"/>
+      <c r="H2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="19" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="26"/>
-      <c r="H3" s="18" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="22"/>
+      <c r="H3" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
-      <c r="N3" s="21" t="s">
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="35"/>
+      <c r="N3" s="18" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7570,7 +7585,7 @@
       <c r="E4" s="17">
         <v>2</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>75</v>
       </c>
       <c r="G4">
@@ -7616,7 +7631,7 @@
       <c r="E5" s="17">
         <v>2</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>74</v>
       </c>
       <c r="G5">
@@ -7662,7 +7677,7 @@
       <c r="E6" s="17">
         <v>2</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="23"/>
       <c r="H6" s="15" t="s">
         <v>69</v>
       </c>
@@ -7680,14 +7695,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="22"/>
       <c r="H7" s="15" t="s">
         <v>70</v>
       </c>
@@ -7720,7 +7735,7 @@
       <c r="E8" s="17">
         <v>18</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="23" t="s">
         <v>75</v>
       </c>
       <c r="G8">
@@ -7759,22 +7774,22 @@
       <c r="E9" s="17">
         <v>18</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="23" t="s">
         <v>74</v>
       </c>
       <c r="G9">
         <f>AVERAGE(B10:B11)</f>
         <v>17.664999999999999</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="18" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7794,7 +7809,7 @@
       <c r="E10" s="17">
         <v>14</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="23"/>
       <c r="H10" s="15" t="s">
         <v>67</v>
       </c>
@@ -7834,7 +7849,7 @@
       <c r="E11" s="17">
         <v>16</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="23"/>
       <c r="H11" s="15" t="s">
         <v>68</v>
       </c>
@@ -7859,14 +7874,14 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="26"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="22"/>
       <c r="H12" s="15" t="s">
         <v>69</v>
       </c>
@@ -7899,7 +7914,7 @@
       <c r="E13" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="23" t="s">
         <v>75</v>
       </c>
       <c r="G13">
@@ -7938,7 +7953,7 @@
       <c r="E14" s="17">
         <v>3</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="23" t="s">
         <v>74</v>
       </c>
       <c r="G14">
@@ -7977,8 +7992,8 @@
       <c r="E15" s="17">
         <v>2</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="H15" s="24" t="s">
+      <c r="F15" s="23"/>
+      <c r="H15" s="20" t="s">
         <v>75</v>
       </c>
       <c r="I15">
@@ -7990,15 +8005,15 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="26"/>
-      <c r="H16" s="24" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="22"/>
+      <c r="H16" s="20" t="s">
         <v>74</v>
       </c>
       <c r="I16">
@@ -8025,7 +8040,7 @@
       <c r="E17" s="17">
         <v>33</v>
       </c>
-      <c r="F17" s="27"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -8043,7 +8058,7 @@
       <c r="E18" s="17">
         <v>33</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="23" t="s">
         <v>75</v>
       </c>
       <c r="G18">
@@ -8067,7 +8082,7 @@
       <c r="E19" s="17">
         <v>25</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="23" t="s">
         <v>74</v>
       </c>
       <c r="G19">
@@ -8091,26 +8106,26 @@
       <c r="E20" s="17">
         <v>31</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B21">
         <f>AVERAGE(G4,G8,G13,G18)</f>
         <v>29.392499999999998</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="20"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="35"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B22">
@@ -8169,13 +8184,13 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
@@ -8212,13 +8227,13 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
@@ -8255,7 +8270,7 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B33">
@@ -8264,7 +8279,7 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B34">
@@ -8281,17 +8296,17 @@
       </c>
     </row>
     <row r="37" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20"/>
-      <c r="H37" s="28" t="s">
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
+      <c r="H37" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8367,13 +8382,13 @@
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="35"/>
       <c r="H41">
         <f>H38+B46</f>
         <v>120.32499999999999</v>
@@ -8439,29 +8454,29 @@
       <c r="E44" s="17">
         <v>30</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="20"/>
-      <c r="N44" s="18" t="s">
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="35"/>
+      <c r="N44" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="20"/>
+      <c r="O44" s="34"/>
+      <c r="P44" s="34"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="35"/>
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="20"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="35"/>
       <c r="H45" s="15" t="s">
         <v>78</v>
       </c>
@@ -8477,7 +8492,7 @@
       <c r="L45" s="17">
         <v>33</v>
       </c>
-      <c r="M45" s="27"/>
+      <c r="M45" s="23"/>
       <c r="N45" s="15" t="s">
         <v>33</v>
       </c>
@@ -8532,7 +8547,7 @@
       <c r="L46" s="17">
         <v>33</v>
       </c>
-      <c r="M46" s="27"/>
+      <c r="M46" s="23"/>
       <c r="N46" s="15" t="s">
         <v>70</v>
       </c>
@@ -8612,22 +8627,22 @@
       <c r="E48" s="17">
         <v>52</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="20"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="35"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="20"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="35"/>
       <c r="H49" s="15" t="s">
         <v>78</v>
       </c>
@@ -8724,7 +8739,7 @@
       <c r="E52" s="17">
         <v>19</v>
       </c>
-      <c r="H52" s="24" t="s">
+      <c r="H52" s="20" t="s">
         <v>75</v>
       </c>
       <c r="I52">
@@ -8748,7 +8763,7 @@
       <c r="E53" s="17">
         <v>19</v>
       </c>
-      <c r="H53" s="24" t="s">
+      <c r="H53" s="20" t="s">
         <v>74</v>
       </c>
       <c r="I53">
@@ -8775,23 +8790,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H9:L9"/>
     <mergeCell ref="A45:E45"/>
     <mergeCell ref="A49:E49"/>
     <mergeCell ref="H44:L44"/>
     <mergeCell ref="H48:L48"/>
     <mergeCell ref="N44:R44"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="H9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WORK IN PROGRESS. This commit adds an appliance calibration script. The script compiles, but has not been allowed to run to completion. This is just a nightly commit to backup
</commit_message>
<xml_diff>
--- a/bcd/CREST/Appliance/Appliance_Characteristics.xlsx
+++ b/bcd/CREST/Appliance/Appliance_Characteristics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="99">
   <si>
     <t>Appliance Name</t>
   </si>
@@ -310,13 +310,16 @@
   </si>
   <si>
     <t>Ready</t>
+  </si>
+  <si>
+    <t>Once a week/15 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +384,13 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -553,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -607,7 +617,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -621,6 +630,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2880,11 +2893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64158336"/>
-        <c:axId val="64512384"/>
+        <c:axId val="40493056"/>
+        <c:axId val="42166912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64158336"/>
+        <c:axId val="40493056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="365"/>
@@ -2896,12 +2909,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64512384"/>
+        <c:crossAx val="42166912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64512384"/>
+        <c:axId val="42166912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,7 +2925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64158336"/>
+        <c:crossAx val="40493056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3259,7 +3272,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,6 +3366,9 @@
       <c r="C3" s="6">
         <v>3500</v>
       </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
       <c r="E3" s="8">
         <v>16</v>
       </c>
@@ -3389,6 +3405,9 @@
       <c r="C4" s="6">
         <v>3200</v>
       </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
       <c r="E4" s="8">
         <v>27</v>
       </c>
@@ -3425,6 +3444,9 @@
       <c r="C5" s="4">
         <v>1300</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5" s="9">
         <v>124</v>
       </c>
@@ -3458,6 +3480,9 @@
       <c r="C6" s="9">
         <v>5535</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="E6" s="9">
         <v>75</v>
       </c>
@@ -3491,7 +3516,12 @@
       <c r="C7" s="4">
         <v>500</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>40</v>
+      </c>
       <c r="F7" s="10">
         <v>211</v>
       </c>
@@ -3501,15 +3531,15 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11.722222222222221</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.8611111111111107</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3522,7 +3552,10 @@
       <c r="C8" s="4">
         <v>100</v>
       </c>
-      <c r="E8" s="5">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10">
         <v>122</v>
       </c>
       <c r="F8" s="8">
@@ -3558,7 +3591,7 @@
       <c r="D9" s="14">
         <v>3.3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="10">
         <v>122</v>
       </c>
       <c r="F9" s="8">
@@ -3630,23 +3663,27 @@
       <c r="D11" s="26">
         <v>0</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="E11" s="29">
+        <v>20</v>
+      </c>
+      <c r="F11" s="29">
+        <v>52</v>
+      </c>
       <c r="G11" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="H11" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4444444444444442</v>
       </c>
       <c r="J11" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3656,13 +3693,15 @@
       <c r="B12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>120</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>4</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="29">
+        <v>150</v>
+      </c>
       <c r="F12" s="29">
         <v>449</v>
       </c>
@@ -3672,41 +3711,41 @@
       </c>
       <c r="H12" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I12" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>93.541666666666671</v>
       </c>
       <c r="J12" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11.225</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="26">
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J13" s="39">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3796,23 +3835,30 @@
       <c r="D16" s="28">
         <v>0</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="29">
+        <v>15</v>
+      </c>
+      <c r="F16" s="29">
+        <v>52</v>
+      </c>
       <c r="G16" s="26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="H16" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.75</v>
       </c>
       <c r="I16" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="J16" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11.916666666666666</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4008,7 +4054,7 @@
       <c r="D22" s="14">
         <v>26</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="10">
         <v>122</v>
       </c>
       <c r="F22" s="8">
@@ -4083,12 +4129,12 @@
       <c r="E24" s="5">
         <v>5</v>
       </c>
-      <c r="F24" s="4">
-        <v>864</v>
+      <c r="F24" s="5">
+        <v>365</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>30.416666666666668</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
@@ -4096,11 +4142,11 @@
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="J24" s="4">
+        <v>2.5347222222222223</v>
+      </c>
+      <c r="J24" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>2.5347222222222223</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -4116,21 +4162,27 @@
       <c r="D25" s="14">
         <v>1</v>
       </c>
+      <c r="E25" s="10">
+        <v>50</v>
+      </c>
+      <c r="F25" s="10">
+        <v>365</v>
+      </c>
       <c r="G25" s="11">
         <f t="shared" ref="G25" si="4">F25/12</f>
-        <v>0</v>
+        <v>30.416666666666668</v>
       </c>
       <c r="H25" s="11">
         <f t="shared" ref="H25" si="5">(C25/1000)*(E25/60)</f>
-        <v>0</v>
+        <v>2.0833333333333336E-2</v>
       </c>
       <c r="I25" s="11">
         <f t="shared" ref="I25" si="6">(G25*E25)/60</f>
-        <v>0</v>
+        <v>25.347222222222225</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" ref="J25" si="7">H25*G25</f>
-        <v>0</v>
+        <v>0.63368055555555569</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -7508,13 +7560,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:14" s="11" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
@@ -7550,21 +7602,21 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="22"/>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="35"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="34"/>
       <c r="N3" s="18" t="s">
         <v>62</v>
       </c>
@@ -7695,13 +7747,13 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="22"/>
       <c r="H7" s="15" t="s">
         <v>70</v>
@@ -7781,13 +7833,13 @@
         <f>AVERAGE(B10:B11)</f>
         <v>17.664999999999999</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34"/>
       <c r="M9" s="11"/>
       <c r="N9" s="18" t="s">
         <v>62</v>
@@ -7874,13 +7926,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="22"/>
       <c r="H12" s="15" t="s">
         <v>69</v>
@@ -8005,13 +8057,13 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
       <c r="F16" s="22"/>
       <c r="H16" s="20" t="s">
         <v>74</v>
@@ -8116,13 +8168,13 @@
         <f>AVERAGE(G4,G8,G13,G18)</f>
         <v>29.392499999999998</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
@@ -8184,13 +8236,13 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="35"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
@@ -8227,13 +8279,13 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
@@ -8296,13 +8348,13 @@
       </c>
     </row>
     <row r="37" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="34"/>
       <c r="H37" s="24" t="s">
         <v>91</v>
       </c>
@@ -8382,13 +8434,13 @@
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="35"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34"/>
       <c r="H41">
         <f>H38+B46</f>
         <v>120.32499999999999</v>
@@ -8454,29 +8506,29 @@
       <c r="E44" s="17">
         <v>30</v>
       </c>
-      <c r="H44" s="33" t="s">
+      <c r="H44" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="35"/>
-      <c r="N44" s="33" t="s">
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="34"/>
+      <c r="N44" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="O44" s="34"/>
-      <c r="P44" s="34"/>
-      <c r="Q44" s="34"/>
-      <c r="R44" s="35"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="34"/>
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="34"/>
       <c r="H45" s="15" t="s">
         <v>78</v>
       </c>
@@ -8627,22 +8679,22 @@
       <c r="E48" s="17">
         <v>52</v>
       </c>
-      <c r="H48" s="33" t="s">
+      <c r="H48" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="35"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="34"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="35"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="34"/>
       <c r="H49" s="15" t="s">
         <v>78</v>
       </c>
@@ -8790,11 +8842,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="N44:R44"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="A27:E27"/>
@@ -8802,11 +8854,11 @@
     <mergeCell ref="A37:E37"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="N44:R44"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WORK IN PROGRESS. Reduced the power rating of the stove element
</commit_message>
<xml_diff>
--- a/bcd/CREST/Appliance/Appliance_Characteristics.xlsx
+++ b/bcd/CREST/Appliance/Appliance_Characteristics.xlsx
@@ -147,9 +147,6 @@
     <t>Range/Oven - Bake Element Only</t>
   </si>
   <si>
-    <t>Electric Range (Oven)</t>
-  </si>
-  <si>
     <t>Hours/Month</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>Once a week/15 min</t>
+  </si>
+  <si>
+    <t>Electric Range (Oven) - Large Element</t>
   </si>
 </sst>
 </file>
@@ -618,6 +618,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -630,10 +634,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2893,11 +2893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40493056"/>
-        <c:axId val="42166912"/>
+        <c:axId val="42566016"/>
+        <c:axId val="42567552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40493056"/>
+        <c:axId val="42566016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="365"/>
@@ -2909,12 +2909,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42166912"/>
+        <c:crossAx val="42567552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42166912"/>
+        <c:axId val="42567552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2925,7 +2925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40493056"/>
+        <c:crossAx val="42566016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3272,7 +3272,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,7 +3314,7 @@
         <v>38</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>35</v>
@@ -3364,7 +3364,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="6">
-        <v>3500</v>
+        <v>2300</v>
       </c>
       <c r="D3" s="8">
         <v>1</v>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>0.93333333333333335</v>
+        <v>0.61333333333333329</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
@@ -3389,10 +3389,10 @@
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J24" si="3">H3*G3</f>
-        <v>44.644444444444446</v>
+        <v>29.337777777777777</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3723,29 +3723,29 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="37">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="35">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>11.916666666666666</v>
       </c>
       <c r="K16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4151,7 +4151,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>12</v>
@@ -4193,7 +4193,7 @@
         <v>41</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -4206,25 +4206,25 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -7560,70 +7560,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H1" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="H1" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
     </row>
     <row r="2" spans="1:14" s="11" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>64</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>65</v>
       </c>
       <c r="F2" s="21"/>
       <c r="H2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="19" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="22"/>
+      <c r="H3" s="36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="22"/>
-      <c r="H3" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
       <c r="N3" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="16">
         <v>44.63</v>
@@ -7638,14 +7638,14 @@
         <v>2</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4">
         <f>AVERAGE(B4:B5)</f>
         <v>44.515000000000001</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" s="16">
         <v>13.99</v>
@@ -7660,7 +7660,7 @@
         <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N4">
         <f>AVERAGE(I4:I6,I8)</f>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="5" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="16">
         <v>44.4</v>
@@ -7684,14 +7684,14 @@
         <v>2</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5">
         <f>B6</f>
         <v>43.46</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="16">
         <v>13.85</v>
@@ -7706,7 +7706,7 @@
         <v>24</v>
       </c>
       <c r="M5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N5">
         <f>I7</f>
@@ -7715,7 +7715,7 @@
     </row>
     <row r="6" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="16">
         <v>43.46</v>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="F6" s="23"/>
       <c r="H6" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" s="16">
         <v>19.09</v>
@@ -7747,16 +7747,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="22"/>
       <c r="H7" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" s="16">
         <v>8.32</v>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="8" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="16">
         <v>24.65</v>
@@ -7788,14 +7788,14 @@
         <v>18</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8">
         <f>AVERAGE(B8:B9)</f>
         <v>27.145</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="16">
         <v>14.41</v>
@@ -7812,7 +7812,7 @@
     </row>
     <row r="9" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="16">
         <v>29.64</v>
@@ -7827,27 +7827,27 @@
         <v>18</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9">
         <f>AVERAGE(B10:B11)</f>
         <v>17.664999999999999</v>
       </c>
-      <c r="H9" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="34"/>
+      <c r="H9" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="38"/>
       <c r="M9" s="11"/>
       <c r="N9" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="16">
         <v>17.829999999999998</v>
@@ -7863,7 +7863,7 @@
       </c>
       <c r="F10" s="23"/>
       <c r="H10" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="16">
         <v>4.1100000000000003</v>
@@ -7878,7 +7878,7 @@
         <v>15</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N10" s="11">
         <f>AVERAGE(I10:I12,I14)</f>
@@ -7887,7 +7887,7 @@
     </row>
     <row r="11" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="16">
         <v>17.5</v>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="F11" s="23"/>
       <c r="H11" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="16">
         <v>2.42</v>
@@ -7918,7 +7918,7 @@
         <v>13</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N11" s="11">
         <f>I13</f>
@@ -7926,16 +7926,16 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
+      <c r="A12" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="22"/>
       <c r="H12" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="16">
         <v>6.8</v>
@@ -7952,7 +7952,7 @@
     </row>
     <row r="13" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="16">
         <v>28.35</v>
@@ -7967,14 +7967,14 @@
         <v>2</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13">
         <f>AVERAGE(B13:B14)</f>
         <v>29.86</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="16">
         <v>1.66</v>
@@ -7991,7 +7991,7 @@
     </row>
     <row r="14" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="16">
         <v>31.37</v>
@@ -8006,14 +8006,14 @@
         <v>3</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14">
         <f>B15</f>
         <v>27.8</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I14" s="16">
         <v>3.3</v>
@@ -8030,7 +8030,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="16">
         <v>27.8</v>
@@ -8046,39 +8046,39 @@
       </c>
       <c r="F15" s="23"/>
       <c r="H15" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I15">
         <f>AVERAGE(N4,N10)</f>
         <v>9.7462499999999999</v>
       </c>
       <c r="J15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
+      <c r="A16" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="22"/>
       <c r="H16" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I16">
         <f>AVERAGE(N5,N11)</f>
         <v>4.99</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="16">
         <v>15.95</v>
@@ -8096,7 +8096,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="16">
         <v>16.149999999999999</v>
@@ -8111,7 +8111,7 @@
         <v>33</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18">
         <f>AVERAGE(B17:B18)</f>
@@ -8120,7 +8120,7 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="16">
         <v>15.66</v>
@@ -8135,7 +8135,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19">
         <f>AVERAGE(B19:B20)</f>
@@ -8144,7 +8144,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="16">
         <v>15.47</v>
@@ -8162,30 +8162,30 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <f>AVERAGE(G4,G8,G13,G18)</f>
         <v>29.392499999999998</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="H21" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="34"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="38"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22">
         <f>AVERAGE(G5,G9,G14,G19)</f>
         <v>26.122499999999999</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I22" s="16">
         <v>8.6199999999999992</v>
@@ -8202,7 +8202,7 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I23" s="16">
         <v>9.91</v>
@@ -8219,7 +8219,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H24" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I24" s="16">
         <v>5.04</v>
@@ -8236,17 +8236,17 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
+      <c r="A27" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="16">
         <v>1.26</v>
@@ -8263,7 +8263,7 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="16">
         <v>4.93</v>
@@ -8279,17 +8279,17 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="A30" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="16">
         <v>1.58</v>
@@ -8306,7 +8306,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="16">
         <v>131.07</v>
@@ -8323,7 +8323,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33">
         <f>AVERAGE(B29,B32)</f>
@@ -8332,7 +8332,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <f>AVERAGE(B28,B31)</f>
@@ -8341,30 +8341,30 @@
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="34"/>
+      <c r="A37" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="38"/>
       <c r="H37" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="16">
         <v>0.8</v>
@@ -8383,19 +8383,19 @@
         <v>46.354999999999997</v>
       </c>
       <c r="I38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J38">
         <f>AVERAGE(B38,B42)</f>
         <v>0.96499999999999997</v>
       </c>
       <c r="K38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="16">
         <v>65.099999999999994</v>
@@ -8412,7 +8412,7 @@
     </row>
     <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="16">
         <v>12.14</v>
@@ -8427,38 +8427,38 @@
         <v>14</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
+      <c r="A41" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
       <c r="H41">
         <f>H38+B46</f>
         <v>120.32499999999999</v>
       </c>
       <c r="I41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J41">
         <f>B47+J38</f>
         <v>3.8049999999999997</v>
       </c>
       <c r="K41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="16">
         <v>1.1299999999999999</v>
@@ -8475,7 +8475,7 @@
     </row>
     <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="16">
         <v>27.61</v>
@@ -8492,7 +8492,7 @@
     </row>
     <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="16">
         <v>1.38</v>
@@ -8506,31 +8506,31 @@
       <c r="E44" s="17">
         <v>30</v>
       </c>
-      <c r="H44" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="34"/>
-      <c r="N44" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="O44" s="33"/>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="33"/>
-      <c r="R44" s="34"/>
+      <c r="H44" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="38"/>
+      <c r="N44" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="38"/>
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="34"/>
+      <c r="A45" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="38"/>
       <c r="H45" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I45" s="16">
         <v>7.54</v>
@@ -8561,7 +8561,7 @@
         <v>24</v>
       </c>
       <c r="S45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T45">
         <f>AVERAGE(O45,O47)</f>
@@ -8570,7 +8570,7 @@
     </row>
     <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" s="16">
         <v>73.97</v>
@@ -8585,7 +8585,7 @@
         <v>63</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I46" s="16">
         <v>9.91</v>
@@ -8601,7 +8601,7 @@
       </c>
       <c r="M46" s="23"/>
       <c r="N46" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O46" s="16">
         <v>1.01</v>
@@ -8618,7 +8618,7 @@
     </row>
     <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" s="16">
         <v>2.84</v>
@@ -8633,7 +8633,7 @@
         <v>64</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I47" s="16">
         <v>1.55</v>
@@ -8648,7 +8648,7 @@
         <v>33</v>
       </c>
       <c r="N47" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O47" s="16">
         <v>23.34</v>
@@ -8665,7 +8665,7 @@
     </row>
     <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="16">
         <v>21.13</v>
@@ -8679,24 +8679,24 @@
       <c r="E48" s="17">
         <v>52</v>
       </c>
-      <c r="H48" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="34"/>
+      <c r="H48" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="38"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="34"/>
+      <c r="A49" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="38"/>
       <c r="H49" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I49" s="16">
         <v>13.51</v>
@@ -8713,7 +8713,7 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" s="16">
         <v>29.48</v>
@@ -8728,7 +8728,7 @@
         <v>13</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I50" s="16">
         <v>15.33</v>
@@ -8745,7 +8745,7 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" s="16">
         <v>44.28</v>
@@ -8760,7 +8760,7 @@
         <v>8</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I51" s="16">
         <v>5.04</v>
@@ -8777,7 +8777,7 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" s="16">
         <v>8.9</v>
@@ -8792,7 +8792,7 @@
         <v>19</v>
       </c>
       <c r="H52" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I52">
         <f>AVERAGE(I45:I46,I49:I50)</f>
@@ -8801,7 +8801,7 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="16">
         <v>4.42</v>
@@ -8816,7 +8816,7 @@
         <v>19</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I53">
         <f>AVERAGE(I47,I51)</f>
@@ -8825,7 +8825,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="16">
         <v>15.77</v>
@@ -8842,11 +8842,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="N44:R44"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A16:E16"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="A27:E27"/>
@@ -8854,11 +8854,11 @@
     <mergeCell ref="A37:E37"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="N44:R44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>